<commit_message>
adding extra fields to involvement - address, phone, etc. for empi and registar compatibility. closes #3989. closes #3988.
</commit_message>
<xml_diff>
--- a/spec/uploads/excel.xlsx
+++ b/spec/uploads/excel.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
-  <si>
-    <t>mrn</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>case_number</t>
   </si>
@@ -121,6 +118,12 @@
   </si>
   <si>
     <t>Leffler</t>
+  </si>
+  <si>
+    <t>nmff_mrn</t>
+  </si>
+  <si>
+    <t>nmh_mrn</t>
   </si>
 </sst>
 </file>
@@ -157,9 +160,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -490,220 +494,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:N8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1">
+        <v>18995</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1">
+        <v>38414</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1">
-        <v>18995</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
+    <row r="3" spans="1:15">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1">
-        <v>38414</v>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1">
+        <v>11079</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="1">
+        <v>38415</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1">
-        <v>11079</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="1">
-        <v>38415</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>12125</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="L4" s="1">
+        <v>38416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="K4" s="1">
+      <c r="J5" s="3"/>
+      <c r="L5" s="1">
+        <v>38417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1">
+        <v>36770</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="N6" s="1">
+        <v>38418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1">
+        <v>27184</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="N7" s="1">
         <v>38416</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="B5" t="s">
+    <row r="8" spans="1:15">
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1">
+        <v>23227</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="K5" s="1">
-        <v>38417</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="1">
-        <v>36770</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="M6" s="1">
-        <v>38418</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="1">
-        <v>27184</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="I8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="M7" s="1">
-        <v>38416</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="1">
-        <v>23227</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="M8" s="1">
+      <c r="J8" s="3"/>
+      <c r="N8" s="1">
         <v>38417</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="5">
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>